<commit_message>
Finished ANA1 - Status is TESTING
</commit_message>
<xml_diff>
--- a/Netbeans/ANA-ADDIX/output/data_storge/ainow.xlsx
+++ b/Netbeans/ANA-ADDIX/output/data_storge/ainow.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProjects\Sources\11. ChangeCodeANA\ANA-VIETNAM\Netbeans\ANA-ADDIX\output\data_storge\"/>
     </mc:Choice>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="963">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="1003">
   <si>
     <t>Url</t>
   </si>
@@ -2926,12 +2926,133 @@
   </si>
   <si>
     <t>https://ainow.ai/2019/10/23/180121/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/11/25/181157/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/11/20/181109/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/11/20/181105/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/11/20/181096/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/11/20/180352/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/11/19/180997/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/11/19/180379/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/11/18/180975/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/11/18/180958/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/11/18/180961/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/11/18/180936/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/11/18/180949/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/11/14/180803/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/11/14/180805/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/11/14/180757/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/11/14/180721/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/11/13/180796/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/11/13/180323/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/11/12/180479/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/11/09/180524/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/09/30/175475/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/06/13/172100/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/06/09/171839/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/06/07/171703/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/06/04/171382/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/05/30/170999/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/05/29/170919/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/05/29/170915/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/05/29/170910/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/05/24/170530/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/05/22/170362/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/05/20/170150/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/05/20/170141/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/05/16/169893/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/05/15/169799/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/05/15/169797/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/05/15/169796/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/05/12/169562/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/05/08/169194/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/04/27/168687/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3331,7 +3452,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:A42"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="H34" sqref="H34"/>
@@ -3339,7 +3460,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -3450,6 +3571,106 @@
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>982</v>
       </c>
     </row>
   </sheetData>
@@ -3468,7 +3689,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -3976,7 +4197,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -4819,7 +5040,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -5262,7 +5483,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -5805,7 +6026,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -6093,7 +6314,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -6679,7 +6900,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -6717,7 +6938,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -6943,7 +7164,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -6963,7 +7184,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:A42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
@@ -6971,7 +7192,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -7082,6 +7303,106 @@
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>1002</v>
       </c>
     </row>
   </sheetData>
@@ -7099,7 +7420,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -7177,7 +7498,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -7475,7 +7796,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -8543,7 +8864,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -8826,7 +9147,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -9222,7 +9543,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -9250,7 +9571,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>